<commit_message>
Fix test case 6, 7, 8
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -372,33 +372,6 @@
     <t>L'applicativo non gestisce alcune sezioni opzionali</t>
   </si>
   <si>
-    <t>2023-02-09T16:12:32Z</t>
-  </si>
-  <si>
-    <t>5a7c9502eae94353</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.3c9580e89dfc8ee90f9594bbc6797e13e95777e281f776721460405d74e90bfc.f99e9b229c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.70073af09e34df4005c52f39dece35c5f7521e873bbb0710cb5a3ee0117438ec.075f6e6f21^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.9346559f40dc162c1ab01a9abdb1536e7fdb75132991de677857b888ddb4bdfe.a8f9472025^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>123cc134ab856aae</t>
-  </si>
-  <si>
-    <t>b84f67f691b3b1d8</t>
-  </si>
-  <si>
-    <t>2023-02-09T16:14:39Z</t>
-  </si>
-  <si>
-    <t>2023-02-09T16:18:42Z</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -518,6 +491,33 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.229bc28a9d448511177c0ac3c7954661e30e7d18fe1ee373b55c0ff9ecac38eb.1be4ae4a13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-13T09:03:54Z</t>
+  </si>
+  <si>
+    <t>2023-03-13T10:03:20Z</t>
+  </si>
+  <si>
+    <t>2023-03-13T10:03:37Z</t>
+  </si>
+  <si>
+    <t>3982391fafc63b42</t>
+  </si>
+  <si>
+    <t>6f76db9cb6559af3</t>
+  </si>
+  <si>
+    <t>59d779c685663f3f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d432d578260b3769f32d852d1f1fe3f24f26f5cfbe1cc19af51f5f998e152bfe.8191f6c229^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d432d578260b3769f32d852d1f1fe3f24f26f5cfbe1cc19af51f5f998e152bfe.30d680210f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d432d578260b3769f32d852d1f1fe3f24f26f5cfbe1cc19af51f5f998e152bfe.2abcd58ce0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1376,16 +1376,16 @@
         <v>44</v>
       </c>
       <c r="F10" s="14">
-        <v>44966</v>
+        <v>44998</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16" t="s">
@@ -1415,16 +1415,16 @@
         <v>45</v>
       </c>
       <c r="F11" s="14">
-        <v>44966</v>
+        <v>44998</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="16" t="s">
@@ -1454,16 +1454,16 @@
         <v>46</v>
       </c>
       <c r="F12" s="14">
-        <v>44966</v>
+        <v>44998</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16" t="s">
@@ -1527,16 +1527,16 @@
         <v>44979</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>23</v>
@@ -1570,16 +1570,16 @@
         <v>44979</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>23</v>
@@ -1613,12 +1613,12 @@
         <v>44966</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>23</v>
@@ -1652,16 +1652,16 @@
         <v>44970</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>23</v>
@@ -1695,16 +1695,16 @@
         <v>44971</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>23</v>
@@ -1717,7 +1717,7 @@
         <v>23</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="75.75" thickBot="1">
@@ -1740,16 +1740,16 @@
         <v>44970</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>23</v>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="N20" s="17" t="s">
         <v>23</v>
@@ -1816,16 +1816,16 @@
         <v>44970</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>23</v>
@@ -1859,16 +1859,16 @@
         <v>44970</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>23</v>
@@ -1902,16 +1902,16 @@
         <v>44971</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>23</v>
@@ -1945,16 +1945,16 @@
         <v>44971</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>23</v>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N25" s="17" t="s">
         <v>23</v>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="L26" s="16"/>
       <c r="M26" s="16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N26" s="17" t="s">
         <v>23</v>
@@ -2054,16 +2054,16 @@
         <v>44971</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>23</v>
@@ -2089,7 +2089,7 @@
         <v>40</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="15"/>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L28" s="16"/>
       <c r="M28" s="16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N28" s="17" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Aggiunti dettagli gestione errori
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -385,15 +385,6 @@
     <t>Non gestita dall'applicativo</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore di sintassi.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Campo token JWT non valido.</t>
-  </si>
-  <si>
     <t>2023-02-13T16:40:39Z</t>
   </si>
   <si>
@@ -431,9 +422,6 @@
   </si>
   <si>
     <t>Il codice fiscale viene convertito in caratteri maiuscoli nel CDA automaticamente dal programma</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: il servizio ha impiegato troppo tempo a rispondere</t>
   </si>
   <si>
     <t>Se il comune di residenza non è presente, l'indirizzo di residenza del paziente non viene inserito nel CDA</t>
@@ -475,9 +463,6 @@
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.00e0402b75b4bcf5ff3a5d1dbf9b67d4c6bbbae0857d9e96402c83475bfa76d5.08807e0a4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore vocabolario.</t>
-  </si>
-  <si>
     <t>2023-02-22T11:49:27Z</t>
   </si>
   <si>
@@ -503,6 +488,31 @@
   </si>
   <si>
     <t>L'applicativo non gestisce alcune sezioni opzionali nel dettaglio richiesto</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Campo token JWT non valido.
+L'errore viene segnalato all'utente.
+Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: il servizio ha impiegato troppo tempo a rispondere.
+L'errore viene segnalato all'utente.
+In questo caso il documento viene comunque fatto firmare e pubblicato. Si potrà decidere con il cliente se impostare re-invii automatici o manuali.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore di sintassi.
+L'errore viene segnalato all'utente.
+Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore semantico.
+L'errore viene segnalato all'utente.
+Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore vocabolario.
+L'errore viene segnalato all'utente.
+Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1152,10 @@
   <dimension ref="A1:O873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1364,13 +1374,13 @@
         <v>45009</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16" t="s">
@@ -1409,7 +1419,7 @@
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="N11" s="17"/>
       <c r="O11" s="18"/>
@@ -1440,7 +1450,7 @@
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="N12" s="17"/>
       <c r="O12" s="18"/>
@@ -1476,7 +1486,7 @@
       <c r="N13" s="17"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:15" ht="90.75" thickBot="1">
+    <row r="14" spans="1:15" ht="135.75" thickBot="1">
       <c r="A14" s="11">
         <v>29</v>
       </c>
@@ -1496,16 +1506,16 @@
         <v>44979</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>64</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>23</v>
@@ -1519,7 +1529,7 @@
       </c>
       <c r="O14" s="18"/>
     </row>
-    <row r="15" spans="1:15" ht="105.75" thickBot="1">
+    <row r="15" spans="1:15" ht="135.75" thickBot="1">
       <c r="A15" s="11">
         <v>37</v>
       </c>
@@ -1539,16 +1549,16 @@
         <v>44979</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I15" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>23</v>
@@ -1562,7 +1572,7 @@
       </c>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1">
+    <row r="16" spans="1:15" ht="90.75" thickBot="1">
       <c r="A16" s="11">
         <v>45</v>
       </c>
@@ -1587,7 +1597,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="16" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>23</v>
@@ -1601,7 +1611,7 @@
       </c>
       <c r="O16" s="18"/>
     </row>
-    <row r="17" spans="1:15" ht="75.75" thickBot="1">
+    <row r="17" spans="1:15" ht="135.75" thickBot="1">
       <c r="A17" s="11">
         <v>63</v>
       </c>
@@ -1621,16 +1631,16 @@
         <v>44970</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>23</v>
@@ -1644,7 +1654,7 @@
       </c>
       <c r="O17" s="18"/>
     </row>
-    <row r="18" spans="1:15" ht="75.75" thickBot="1">
+    <row r="18" spans="1:15" ht="135.75" thickBot="1">
       <c r="A18" s="11">
         <v>64</v>
       </c>
@@ -1664,16 +1674,16 @@
         <v>44971</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>23</v>
@@ -1686,10 +1696,10 @@
         <v>23</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="75.75" thickBot="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="135.75" thickBot="1">
       <c r="A19" s="11">
         <v>65</v>
       </c>
@@ -1709,16 +1719,16 @@
         <v>44970</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>23</v>
@@ -1758,14 +1768,14 @@
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N20" s="17" t="s">
         <v>23</v>
       </c>
       <c r="O20" s="18"/>
     </row>
-    <row r="21" spans="1:15" ht="75.75" thickBot="1">
+    <row r="21" spans="1:15" ht="135.75" thickBot="1">
       <c r="A21" s="11">
         <v>67</v>
       </c>
@@ -1785,16 +1795,16 @@
         <v>44970</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>23</v>
@@ -1808,7 +1818,7 @@
       </c>
       <c r="O21" s="18"/>
     </row>
-    <row r="22" spans="1:15" ht="75.75" thickBot="1">
+    <row r="22" spans="1:15" ht="135.75" thickBot="1">
       <c r="A22" s="11">
         <v>68</v>
       </c>
@@ -1828,16 +1838,16 @@
         <v>44970</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>23</v>
@@ -1851,7 +1861,7 @@
       </c>
       <c r="O22" s="18"/>
     </row>
-    <row r="23" spans="1:15" ht="75.75" thickBot="1">
+    <row r="23" spans="1:15" ht="135.75" thickBot="1">
       <c r="A23" s="11">
         <v>69</v>
       </c>
@@ -1871,16 +1881,16 @@
         <v>44971</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>23</v>
@@ -1894,7 +1904,7 @@
       </c>
       <c r="O23" s="18"/>
     </row>
-    <row r="24" spans="1:15" ht="75.75" thickBot="1">
+    <row r="24" spans="1:15" ht="135.75" thickBot="1">
       <c r="A24" s="11">
         <v>70</v>
       </c>
@@ -1914,16 +1924,16 @@
         <v>44971</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>23</v>
@@ -2003,7 +2013,7 @@
       </c>
       <c r="O26" s="18"/>
     </row>
-    <row r="27" spans="1:15" ht="75.75" thickBot="1">
+    <row r="27" spans="1:15" ht="135.75" thickBot="1">
       <c r="A27" s="11">
         <v>73</v>
       </c>
@@ -2023,16 +2033,16 @@
         <v>44971</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Valorizzate colonne H, L, M, O, P
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="219">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -488,31 +488,6 @@
     <t>L'applicativo non gestisce alcune sezioni opzionali nel dettaglio richiesto</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Campo token JWT non valido.
-L'errore viene segnalato all'utente.
-Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: il servizio ha impiegato troppo tempo a rispondere.
-L'errore viene segnalato all'utente.
-In questo caso il documento viene comunque fatto firmare e pubblicato. Si potrà decidere con il cliente se impostare re-invii automatici o manuali.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore di sintassi.
-L'errore viene segnalato all'utente.
-Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore semantico.
-L'errore viene segnalato all'utente.
-Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore vocabolario.
-L'errore viene segnalato all'utente.
-Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
-  </si>
-  <si>
     <t>ERRORE BLOCCANTE (SI/NO)</t>
   </si>
   <si>
@@ -867,21 +842,12 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.45c976e65f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Campo token JWT non valido. (Il campo purpose_of_use non è valorizzato)</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Campo token JWT non valido. (Il campo action_id non è corretto)</t>
-  </si>
-  <si>
     <t>2023-11-22T16:25:58Z</t>
   </si>
   <si>
     <t>12331bad019decf1</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Campo token JWT non valido. (Il codice fiscale nel campo person_id non è corretto)</t>
-  </si>
-  <si>
     <t>2023-11-22T16:29:53Z</t>
   </si>
   <si>
@@ -891,12 +857,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.c34ce324be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-6| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'])</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore di sintassi. (ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.)</t>
-  </si>
-  <si>
     <t>2023-11-22T16:43:40Z</t>
   </si>
   <si>
@@ -906,9 +866,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.c7310c0edd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'])</t>
-  </si>
-  <si>
     <t>2023-11-22T16:47:09Z</t>
   </si>
   <si>
@@ -927,12 +884,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.f7d467fca5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-33a| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR' ])</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore vocabolario. (Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: N])</t>
-  </si>
-  <si>
     <t>2023-11-22T16:55:35Z</t>
   </si>
   <si>
@@ -942,9 +893,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.b0b9e9f44d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-38| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ])</t>
-  </si>
-  <si>
     <t>2023-11-22T16:58:03Z</t>
   </si>
   <si>
@@ -954,9 +902,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.f09e4c936c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore di sintassi. (ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.)</t>
-  </si>
-  <si>
     <t>2023-11-22T17:01:27Z</t>
   </si>
   <si>
@@ -966,9 +911,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.60d1376210^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore di sintassi. (ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.,ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.)</t>
-  </si>
-  <si>
     <t>2023-11-22T17:05:05Z</t>
   </si>
   <si>
@@ -978,9 +920,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.3d12239114^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore di sintassi. (ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element 'component' is not complete. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":section}' is expected.)</t>
-  </si>
-  <si>
     <t>2023-11-22T17:08:20Z</t>
   </si>
   <si>
@@ -990,9 +929,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.7ab1d39009^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry']","status":422,"instance":"/validation/error","workflowInstanceId":"2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.7ab1d39009^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"})</t>
-  </si>
-  <si>
     <t>2023-11-22T17:12:22Z</t>
   </si>
   <si>
@@ -1000,9 +936,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.e9f4cb1793^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Errore validazione CDA: Errore semantico. ([ERRORE-30| L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice \"S\" ])</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT0</t>
@@ -1020,6 +953,18 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.71eaa9b8d1160b47b16fe7e7df5da03043290604cfcd4d16257cd4b48cfdf547.10b55eb072^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Campo token JWT non valido.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore di sintassi.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore semantico.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore vocabolario.</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1508,10 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
@@ -1792,10 +1737,10 @@
   <dimension ref="A1:T872"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2027,16 +1972,16 @@
         <v>14</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M9" s="28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>11</v>
@@ -2051,7 +1996,7 @@
         <v>16</v>
       </c>
       <c r="T9" s="33" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="135.75" thickBot="1">
@@ -2097,7 +2042,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
       <c r="T10" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="135.75" thickBot="1">
@@ -2135,7 +2080,7 @@
       <c r="R11" s="17"/>
       <c r="S11" s="18"/>
       <c r="T11" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="135.75" thickBot="1">
@@ -2173,7 +2118,7 @@
       <c r="R12" s="17"/>
       <c r="S12" s="18"/>
       <c r="T12" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="135.75" thickBot="1">
@@ -2211,7 +2156,7 @@
       <c r="R13" s="17"/>
       <c r="S13" s="18"/>
       <c r="T13" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="120.75" thickBot="1">
@@ -2246,22 +2191,28 @@
         <v>23</v>
       </c>
       <c r="K14" s="16"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="16" t="s">
-        <v>103</v>
+      <c r="L14" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="O14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R14" s="41"/>
       <c r="S14" s="18"/>
       <c r="T14" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="135.75" thickBot="1">
@@ -2296,25 +2247,31 @@
         <v>23</v>
       </c>
       <c r="K15" s="16"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="16" t="s">
-        <v>103</v>
+      <c r="L15" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="O15" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q15" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R15" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R15" s="41"/>
       <c r="S15" s="18"/>
       <c r="T15" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="90.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="30.75" thickBot="1">
       <c r="A16" s="11">
         <v>45</v>
       </c>
@@ -2341,13 +2298,13 @@
       <c r="J16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
       <c r="P16" s="40" t="s">
-        <v>104</v>
+        <v>173</v>
       </c>
       <c r="Q16" s="16" t="s">
         <v>41</v>
@@ -2357,10 +2314,10 @@
       </c>
       <c r="S16" s="18"/>
       <c r="T16" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="105.75" thickBot="1">
       <c r="A17" s="11">
         <v>63</v>
       </c>
@@ -2392,25 +2349,31 @@
         <v>23</v>
       </c>
       <c r="K17" s="16"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="16" t="s">
-        <v>105</v>
+      <c r="L17" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="O17" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R17" s="41"/>
       <c r="S17" s="18"/>
       <c r="T17" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="105.75" thickBot="1">
       <c r="A18" s="11">
         <v>64</v>
       </c>
@@ -2442,27 +2405,33 @@
         <v>23</v>
       </c>
       <c r="K18" s="16"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="16" t="s">
-        <v>106</v>
+      <c r="L18" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M18" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="O18" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P18" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R18" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R18" s="41"/>
       <c r="S18" s="18" t="s">
         <v>80</v>
       </c>
       <c r="T18" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="105.75" thickBot="1">
       <c r="A19" s="11">
         <v>65</v>
       </c>
@@ -2494,22 +2463,28 @@
         <v>23</v>
       </c>
       <c r="K19" s="16"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="16" t="s">
-        <v>106</v>
+      <c r="L19" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="O19" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R19" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R19" s="41"/>
       <c r="S19" s="18"/>
       <c r="T19" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="105.75" thickBot="1">
@@ -2544,15 +2519,13 @@
       <c r="O20" s="26"/>
       <c r="P20" s="16"/>
       <c r="Q20" s="16"/>
-      <c r="R20" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R20" s="41"/>
       <c r="S20" s="18"/>
       <c r="T20" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="105.75" thickBot="1">
       <c r="A21" s="11">
         <v>67</v>
       </c>
@@ -2584,25 +2557,31 @@
         <v>23</v>
       </c>
       <c r="K21" s="16"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="40" t="s">
-        <v>106</v>
+      <c r="L21" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N21" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="O21" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R21" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R21" s="41"/>
       <c r="S21" s="18"/>
       <c r="T21" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="105.75" thickBot="1">
       <c r="A22" s="11">
         <v>68</v>
       </c>
@@ -2634,25 +2613,31 @@
         <v>23</v>
       </c>
       <c r="K22" s="16"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="16" t="s">
-        <v>105</v>
+      <c r="L22" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="O22" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q22" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R22" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R22" s="41"/>
       <c r="S22" s="18"/>
       <c r="T22" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="105.75" thickBot="1">
       <c r="A23" s="11">
         <v>69</v>
       </c>
@@ -2684,25 +2669,31 @@
         <v>23</v>
       </c>
       <c r="K23" s="16"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="16" t="s">
-        <v>106</v>
+      <c r="L23" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N23" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="O23" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q23" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R23" s="41"/>
       <c r="S23" s="18"/>
       <c r="T23" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="105.75" thickBot="1">
       <c r="A24" s="11">
         <v>70</v>
       </c>
@@ -2734,22 +2725,28 @@
         <v>23</v>
       </c>
       <c r="K24" s="16"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="16" t="s">
-        <v>106</v>
+      <c r="L24" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="O24" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q24" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R24" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R24" s="41"/>
       <c r="S24" s="18"/>
       <c r="T24" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="105.75" thickBot="1">
@@ -2784,12 +2781,10 @@
       <c r="O25" s="26"/>
       <c r="P25" s="16"/>
       <c r="Q25" s="16"/>
-      <c r="R25" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R25" s="41"/>
       <c r="S25" s="18"/>
       <c r="T25" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="105.75" thickBot="1">
@@ -2824,15 +2819,13 @@
       <c r="O26" s="26"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
-      <c r="R26" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R26" s="41"/>
       <c r="S26" s="18"/>
       <c r="T26" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="105.75" thickBot="1">
       <c r="A27" s="11">
         <v>73</v>
       </c>
@@ -2864,20 +2857,26 @@
         <v>23</v>
       </c>
       <c r="K27" s="16"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="16" t="s">
-        <v>107</v>
+      <c r="L27" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="N27" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="O27" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="Q27" s="16"/>
-      <c r="R27" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R27" s="41"/>
       <c r="S27" s="18"/>
       <c r="T27" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="105.75" thickBot="1">
@@ -2912,12 +2911,10 @@
       <c r="O28" s="26"/>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="R28" s="41"/>
       <c r="S28" s="18"/>
       <c r="T28" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="150.75" thickBot="1">
@@ -2928,22 +2925,22 @@
         <v>17</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F29" s="38">
         <v>45252</v>
       </c>
       <c r="G29" s="39" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H29" s="39" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I29" s="39" t="s">
         <v>64</v>
@@ -2959,13 +2956,13 @@
         <v>43</v>
       </c>
       <c r="N29" s="40" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="O29" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P29" s="44" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q29" s="40" t="s">
         <v>41</v>
@@ -2973,7 +2970,7 @@
       <c r="R29" s="41"/>
       <c r="S29" s="42"/>
       <c r="T29" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="165.75" thickBot="1">
@@ -2984,22 +2981,22 @@
         <v>17</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F30" s="38">
         <v>45252</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H30" s="39" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I30" s="39" t="s">
         <v>64</v>
@@ -3015,13 +3012,13 @@
         <v>43</v>
       </c>
       <c r="N30" s="40" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="O30" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P30" s="44" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q30" s="40" t="s">
         <v>41</v>
@@ -3029,7 +3026,7 @@
       <c r="R30" s="41"/>
       <c r="S30" s="42"/>
       <c r="T30" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="60.75" thickBot="1">
@@ -3040,19 +3037,19 @@
         <v>17</v>
       </c>
       <c r="C31" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="36" t="s">
-        <v>120</v>
-      </c>
       <c r="E31" s="37" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F31" s="38">
         <v>45252</v>
       </c>
       <c r="G31" s="39" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
@@ -3063,7 +3060,7 @@
       <c r="N31" s="40"/>
       <c r="O31" s="40"/>
       <c r="P31" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="Q31" s="40" t="s">
         <v>41</v>
@@ -3073,7 +3070,7 @@
       </c>
       <c r="S31" s="42"/>
       <c r="T31" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="165.75" thickBot="1">
@@ -3084,25 +3081,25 @@
         <v>17</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F32" s="38">
         <v>45252</v>
       </c>
       <c r="G32" s="39" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H32" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I32" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J32" s="40" t="s">
         <v>23</v>
@@ -3117,7 +3114,7 @@
       <c r="R32" s="41"/>
       <c r="S32" s="42"/>
       <c r="T32" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:20" s="54" customFormat="1" ht="165.75" thickBot="1">
@@ -3128,13 +3125,13 @@
         <v>17</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E33" s="47" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F33" s="48"/>
       <c r="G33" s="49"/>
@@ -3152,10 +3149,10 @@
       <c r="O33" s="50"/>
       <c r="P33" s="50"/>
       <c r="Q33" s="50"/>
-      <c r="R33" s="51"/>
+      <c r="R33" s="41"/>
       <c r="S33" s="52"/>
       <c r="T33" s="53" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="165.75" thickBot="1">
@@ -3166,13 +3163,13 @@
         <v>17</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F34" s="38"/>
       <c r="G34" s="39"/>
@@ -3193,7 +3190,7 @@
       <c r="R34" s="41"/>
       <c r="S34" s="42"/>
       <c r="T34" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="165.75" thickBot="1">
@@ -3204,13 +3201,13 @@
         <v>17</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F35" s="38"/>
       <c r="G35" s="39"/>
@@ -3231,7 +3228,7 @@
       <c r="R35" s="41"/>
       <c r="S35" s="42"/>
       <c r="T35" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:20" s="54" customFormat="1" ht="105.75" thickBot="1">
@@ -3242,25 +3239,25 @@
         <v>17</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D36" s="46" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F36" s="48">
         <v>45252</v>
       </c>
       <c r="G36" s="49" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H36" s="49" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I36" s="49" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="J36" s="50" t="s">
         <v>23</v>
@@ -3273,13 +3270,13 @@
         <v>43</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="O36" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P36" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q36" s="50" t="s">
         <v>41</v>
@@ -3287,7 +3284,7 @@
       <c r="R36" s="51"/>
       <c r="S36" s="52"/>
       <c r="T36" s="53" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="120.75" thickBot="1">
@@ -3298,22 +3295,22 @@
         <v>17</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F37" s="48">
         <v>45252</v>
       </c>
       <c r="G37" s="39" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>64</v>
@@ -3329,13 +3326,13 @@
         <v>43</v>
       </c>
       <c r="N37" s="50" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="O37" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P37" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q37" s="50" t="s">
         <v>41</v>
@@ -3343,7 +3340,7 @@
       <c r="R37" s="41"/>
       <c r="S37" s="42"/>
       <c r="T37" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="120.75" thickBot="1">
@@ -3354,25 +3351,25 @@
         <v>17</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E38" s="37" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F38" s="48">
         <v>45252</v>
       </c>
       <c r="G38" s="39" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H38" s="39" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I38" s="39" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J38" s="40" t="s">
         <v>23</v>
@@ -3385,13 +3382,13 @@
         <v>43</v>
       </c>
       <c r="N38" s="50" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="O38" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P38" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q38" s="50" t="s">
         <v>41</v>
@@ -3399,7 +3396,7 @@
       <c r="R38" s="41"/>
       <c r="S38" s="42"/>
       <c r="T38" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="120.75" thickBot="1">
@@ -3410,13 +3407,13 @@
         <v>17</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F39" s="38"/>
       <c r="G39" s="39"/>
@@ -3437,7 +3434,7 @@
       <c r="R39" s="41"/>
       <c r="S39" s="42"/>
       <c r="T39" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="120.75" thickBot="1">
@@ -3448,25 +3445,25 @@
         <v>17</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F40" s="38">
         <v>45252</v>
       </c>
       <c r="G40" s="39" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H40" s="39" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="J40" s="40" t="s">
         <v>23</v>
@@ -3479,13 +3476,13 @@
         <v>43</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="O40" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P40" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q40" s="50" t="s">
         <v>41</v>
@@ -3493,7 +3490,7 @@
       <c r="R40" s="41"/>
       <c r="S40" s="42"/>
       <c r="T40" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="135.75" thickBot="1">
@@ -3504,25 +3501,25 @@
         <v>17</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F41" s="38">
         <v>45252</v>
       </c>
       <c r="G41" s="39" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H41" s="39" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="I41" s="39" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="J41" s="40" t="s">
         <v>23</v>
@@ -3535,13 +3532,13 @@
         <v>43</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="O41" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P41" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q41" s="50" t="s">
         <v>41</v>
@@ -3549,7 +3546,7 @@
       <c r="R41" s="41"/>
       <c r="S41" s="42"/>
       <c r="T41" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="135.75" thickBot="1">
@@ -3560,25 +3557,25 @@
         <v>17</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F42" s="38">
         <v>45252</v>
       </c>
       <c r="G42" s="39" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="J42" s="40" t="s">
         <v>23</v>
@@ -3591,13 +3588,13 @@
         <v>43</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="O42" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P42" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q42" s="50" t="s">
         <v>41</v>
@@ -3605,7 +3602,7 @@
       <c r="R42" s="41"/>
       <c r="S42" s="42"/>
       <c r="T42" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="135.75" thickBot="1">
@@ -3616,25 +3613,25 @@
         <v>17</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F43" s="38">
         <v>45252</v>
       </c>
       <c r="G43" s="39" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H43" s="39" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="I43" s="39" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="J43" s="40" t="s">
         <v>23</v>
@@ -3647,13 +3644,13 @@
         <v>43</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="O43" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P43" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q43" s="50" t="s">
         <v>41</v>
@@ -3661,7 +3658,7 @@
       <c r="R43" s="41"/>
       <c r="S43" s="42"/>
       <c r="T43" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="120.75" thickBot="1">
@@ -3672,25 +3669,25 @@
         <v>17</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F44" s="38">
         <v>45252</v>
       </c>
       <c r="G44" s="39" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="H44" s="39" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="I44" s="39" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="J44" s="40" t="s">
         <v>23</v>
@@ -3703,13 +3700,13 @@
         <v>43</v>
       </c>
       <c r="N44" s="50" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="O44" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P44" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q44" s="50" t="s">
         <v>41</v>
@@ -3717,10 +3714,10 @@
       <c r="R44" s="41"/>
       <c r="S44" s="42"/>
       <c r="T44" s="43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="165.75" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="120.75" thickBot="1">
       <c r="A45" s="35">
         <v>160</v>
       </c>
@@ -3728,25 +3725,25 @@
         <v>17</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F45" s="38">
         <v>45252</v>
       </c>
       <c r="G45" s="39" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="H45" s="39" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="I45" s="39" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="J45" s="40" t="s">
         <v>23</v>
@@ -3765,7 +3762,7 @@
         <v>23</v>
       </c>
       <c r="P45" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q45" s="50" t="s">
         <v>41</v>
@@ -3773,7 +3770,7 @@
       <c r="R45" s="41"/>
       <c r="S45" s="42"/>
       <c r="T45" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="135.75" thickBot="1">
@@ -3784,25 +3781,25 @@
         <v>17</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E46" s="37" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F46" s="38">
         <v>45252</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="H46" s="39" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="I46" s="39" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="J46" s="40" t="s">
         <v>23</v>
@@ -3815,13 +3812,13 @@
         <v>43</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="O46" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P46" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q46" s="50" t="s">
         <v>41</v>
@@ -3829,7 +3826,7 @@
       <c r="R46" s="41"/>
       <c r="S46" s="42"/>
       <c r="T46" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="135.75" thickBot="1">
@@ -3840,13 +3837,13 @@
         <v>17</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E47" s="37" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F47" s="38"/>
       <c r="G47" s="39"/>
@@ -3867,7 +3864,7 @@
       <c r="R47" s="41"/>
       <c r="S47" s="42"/>
       <c r="T47" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="135.75" thickBot="1">
@@ -3878,25 +3875,25 @@
         <v>17</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E48" s="37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F48" s="38">
         <v>45252</v>
       </c>
       <c r="G48" s="39" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="H48" s="39" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="I48" s="39" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="J48" s="40" t="s">
         <v>23</v>
@@ -3909,13 +3906,13 @@
         <v>43</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="O48" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P48" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q48" s="50" t="s">
         <v>41</v>
@@ -3923,7 +3920,7 @@
       <c r="R48" s="41"/>
       <c r="S48" s="42"/>
       <c r="T48" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="135.75" thickBot="1">
@@ -3934,13 +3931,13 @@
         <v>17</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E49" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F49" s="38"/>
       <c r="G49" s="39"/>
@@ -3961,7 +3958,7 @@
       <c r="R49" s="41"/>
       <c r="S49" s="42"/>
       <c r="T49" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="135.75" thickBot="1">
@@ -3972,13 +3969,13 @@
         <v>17</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E50" s="37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F50" s="38"/>
       <c r="G50" s="39"/>
@@ -3999,7 +3996,7 @@
       <c r="R50" s="41"/>
       <c r="S50" s="42"/>
       <c r="T50" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="135.75" thickBot="1">
@@ -4010,13 +4007,13 @@
         <v>17</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E51" s="37" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F51" s="38"/>
       <c r="G51" s="39"/>
@@ -4037,7 +4034,7 @@
       <c r="R51" s="41"/>
       <c r="S51" s="42"/>
       <c r="T51" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="135.75" thickBot="1">
@@ -4048,13 +4045,13 @@
         <v>17</v>
       </c>
       <c r="C52" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E52" s="37" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F52" s="38"/>
       <c r="G52" s="56"/>
@@ -4075,7 +4072,7 @@
       <c r="R52" s="41"/>
       <c r="S52" s="42"/>
       <c r="T52" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="135.75" thickBot="1">
@@ -4086,13 +4083,13 @@
         <v>17</v>
       </c>
       <c r="C53" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E53" s="37" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F53" s="38"/>
       <c r="G53" s="39"/>
@@ -4113,7 +4110,7 @@
       <c r="R53" s="41"/>
       <c r="S53" s="42"/>
       <c r="T53" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="135.75" thickBot="1">
@@ -4124,25 +4121,25 @@
         <v>17</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E54" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F54" s="38">
         <v>45252</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H54" s="39" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="I54" s="39" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="J54" s="40" t="s">
         <v>23</v>
@@ -4155,13 +4152,13 @@
         <v>43</v>
       </c>
       <c r="N54" s="57" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="O54" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P54" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q54" s="50" t="s">
         <v>41</v>
@@ -4169,7 +4166,7 @@
       <c r="R54" s="41"/>
       <c r="S54" s="42"/>
       <c r="T54" s="43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:20" s="30" customFormat="1" ht="150.75" thickBot="1">
@@ -4183,22 +4180,22 @@
         <v>18</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="F55" s="38">
         <v>45257</v>
       </c>
       <c r="G55" s="39" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="I55" s="39" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="J55" s="40" t="s">
         <v>23</v>
@@ -4215,7 +4212,7 @@
       <c r="R55" s="41"/>
       <c r="S55" s="42"/>
       <c r="T55" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="165">
@@ -4226,25 +4223,25 @@
         <v>17</v>
       </c>
       <c r="C56" s="36" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E56" s="37" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F56" s="38">
         <v>45252</v>
       </c>
       <c r="G56" s="39" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I56" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J56" s="40" t="s">
         <v>23</v>
@@ -4261,7 +4258,7 @@
       <c r="R56" s="41"/>
       <c r="S56" s="42"/>
       <c r="T56" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:20">

</xml_diff>

<commit_message>
Add tests 32, 40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -812,19 +812,7 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.0727f1d404^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-22T14:53:04Z</t>
-  </si>
-  <si>
-    <t>4e04e04ed3c6df79</t>
-  </si>
-  <si>
     <t>Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'utente o all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
-  </si>
-  <si>
-    <t>2023-11-22T16:05:29Z</t>
-  </si>
-  <si>
-    <t>31fc52736b3590f2</t>
   </si>
   <si>
     <t>In questo caso il documento viene comunque fatto firmare e pubblicato. Si potrà decidere con il cliente se impostare re-invii automatici o manuali.</t>
@@ -965,6 +953,18 @@
   </si>
   <si>
     <t>Errore validazione CDA: Errore vocabolario.</t>
+  </si>
+  <si>
+    <t>2023-11-28T17:49:11Z</t>
+  </si>
+  <si>
+    <t>2023-11-28T17:51:35Z</t>
+  </si>
+  <si>
+    <t>e0c3452583586499</t>
+  </si>
+  <si>
+    <t>88051f3d9062deb7</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1737,10 @@
   <dimension ref="A1:T872"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2198,13 +2198,13 @@
         <v>43</v>
       </c>
       <c r="N14" s="40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O14" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P14" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q14" s="16" t="s">
         <v>41</v>
@@ -2254,13 +2254,13 @@
         <v>43</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O15" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P15" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q15" s="16" t="s">
         <v>41</v>
@@ -2304,7 +2304,7 @@
       <c r="N16" s="40"/>
       <c r="O16" s="40"/>
       <c r="P16" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q16" s="16" t="s">
         <v>41</v>
@@ -2356,13 +2356,13 @@
         <v>43</v>
       </c>
       <c r="N17" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O17" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P17" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q17" s="16" t="s">
         <v>41</v>
@@ -2412,13 +2412,13 @@
         <v>43</v>
       </c>
       <c r="N18" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O18" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P18" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q18" s="16" t="s">
         <v>41</v>
@@ -2470,13 +2470,13 @@
         <v>43</v>
       </c>
       <c r="N19" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O19" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P19" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q19" s="16" t="s">
         <v>41</v>
@@ -2564,13 +2564,13 @@
         <v>43</v>
       </c>
       <c r="N21" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O21" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P21" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q21" s="16" t="s">
         <v>41</v>
@@ -2620,13 +2620,13 @@
         <v>43</v>
       </c>
       <c r="N22" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O22" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P22" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q22" s="16" t="s">
         <v>41</v>
@@ -2676,13 +2676,13 @@
         <v>43</v>
       </c>
       <c r="N23" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O23" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P23" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q23" s="16" t="s">
         <v>41</v>
@@ -2732,13 +2732,13 @@
         <v>43</v>
       </c>
       <c r="N24" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O24" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P24" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="16" t="s">
         <v>41</v>
@@ -2864,13 +2864,13 @@
         <v>43</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O27" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P27" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q27" s="16"/>
       <c r="R27" s="41"/>
@@ -2934,13 +2934,13 @@
         <v>112</v>
       </c>
       <c r="F29" s="38">
-        <v>45252</v>
+        <v>45258</v>
       </c>
       <c r="G29" s="39" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="H29" s="39" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="I29" s="39" t="s">
         <v>64</v>
@@ -2956,13 +2956,13 @@
         <v>43</v>
       </c>
       <c r="N29" s="40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O29" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P29" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q29" s="40" t="s">
         <v>41</v>
@@ -2990,13 +2990,13 @@
         <v>114</v>
       </c>
       <c r="F30" s="38">
-        <v>45252</v>
+        <v>45258</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="H30" s="39" t="s">
-        <v>172</v>
+        <v>218</v>
       </c>
       <c r="I30" s="39" t="s">
         <v>64</v>
@@ -3012,13 +3012,13 @@
         <v>43</v>
       </c>
       <c r="N30" s="40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O30" s="40" t="s">
         <v>23</v>
       </c>
       <c r="P30" s="44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q30" s="40" t="s">
         <v>41</v>
@@ -3049,7 +3049,7 @@
         <v>45252</v>
       </c>
       <c r="G31" s="39" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
@@ -3060,7 +3060,7 @@
       <c r="N31" s="40"/>
       <c r="O31" s="40"/>
       <c r="P31" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q31" s="40" t="s">
         <v>41</v>
@@ -3251,13 +3251,13 @@
         <v>45252</v>
       </c>
       <c r="G36" s="49" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H36" s="49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I36" s="49" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J36" s="50" t="s">
         <v>23</v>
@@ -3270,13 +3270,13 @@
         <v>43</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O36" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P36" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q36" s="50" t="s">
         <v>41</v>
@@ -3307,10 +3307,10 @@
         <v>45252</v>
       </c>
       <c r="G37" s="39" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>64</v>
@@ -3326,13 +3326,13 @@
         <v>43</v>
       </c>
       <c r="N37" s="50" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O37" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P37" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q37" s="50" t="s">
         <v>41</v>
@@ -3363,13 +3363,13 @@
         <v>45252</v>
       </c>
       <c r="G38" s="39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H38" s="39" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I38" s="39" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J38" s="40" t="s">
         <v>23</v>
@@ -3382,13 +3382,13 @@
         <v>43</v>
       </c>
       <c r="N38" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O38" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P38" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q38" s="50" t="s">
         <v>41</v>
@@ -3457,13 +3457,13 @@
         <v>45252</v>
       </c>
       <c r="G40" s="39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H40" s="39" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J40" s="40" t="s">
         <v>23</v>
@@ -3476,13 +3476,13 @@
         <v>43</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O40" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P40" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q40" s="50" t="s">
         <v>41</v>
@@ -3513,13 +3513,13 @@
         <v>45252</v>
       </c>
       <c r="G41" s="39" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H41" s="39" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I41" s="39" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J41" s="40" t="s">
         <v>23</v>
@@ -3532,13 +3532,13 @@
         <v>43</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O41" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P41" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q41" s="50" t="s">
         <v>41</v>
@@ -3569,13 +3569,13 @@
         <v>45252</v>
       </c>
       <c r="G42" s="39" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J42" s="40" t="s">
         <v>23</v>
@@ -3588,13 +3588,13 @@
         <v>43</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O42" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P42" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q42" s="50" t="s">
         <v>41</v>
@@ -3625,13 +3625,13 @@
         <v>45252</v>
       </c>
       <c r="G43" s="39" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H43" s="39" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I43" s="39" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J43" s="40" t="s">
         <v>23</v>
@@ -3644,13 +3644,13 @@
         <v>43</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O43" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P43" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q43" s="50" t="s">
         <v>41</v>
@@ -3681,13 +3681,13 @@
         <v>45252</v>
       </c>
       <c r="G44" s="39" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H44" s="39" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I44" s="39" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J44" s="40" t="s">
         <v>23</v>
@@ -3700,13 +3700,13 @@
         <v>43</v>
       </c>
       <c r="N44" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O44" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P44" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q44" s="50" t="s">
         <v>41</v>
@@ -3737,13 +3737,13 @@
         <v>45252</v>
       </c>
       <c r="G45" s="39" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H45" s="39" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I45" s="39" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J45" s="40" t="s">
         <v>23</v>
@@ -3756,13 +3756,13 @@
         <v>43</v>
       </c>
       <c r="N45" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O45" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P45" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q45" s="50" t="s">
         <v>41</v>
@@ -3793,13 +3793,13 @@
         <v>45252</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H46" s="39" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I46" s="39" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J46" s="40" t="s">
         <v>23</v>
@@ -3812,13 +3812,13 @@
         <v>43</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O46" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P46" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q46" s="50" t="s">
         <v>41</v>
@@ -3887,13 +3887,13 @@
         <v>45252</v>
       </c>
       <c r="G48" s="39" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H48" s="39" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I48" s="39" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J48" s="40" t="s">
         <v>23</v>
@@ -3906,13 +3906,13 @@
         <v>43</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O48" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P48" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q48" s="50" t="s">
         <v>41</v>
@@ -4133,13 +4133,13 @@
         <v>45252</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H54" s="39" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I54" s="39" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J54" s="40" t="s">
         <v>23</v>
@@ -4152,13 +4152,13 @@
         <v>43</v>
       </c>
       <c r="N54" s="57" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O54" s="50" t="s">
         <v>23</v>
       </c>
       <c r="P54" s="55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q54" s="50" t="s">
         <v>41</v>
@@ -4180,22 +4180,22 @@
         <v>18</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F55" s="38">
         <v>45257</v>
       </c>
       <c r="G55" s="39" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I55" s="39" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J55" s="40" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Fix case 68, 161
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -650,15 +650,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.60d1376210^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-22T17:05:05Z</t>
-  </si>
-  <si>
-    <t>489b7dce1292b234</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.3d12239114^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-11-22T17:08:20Z</t>
   </si>
   <si>
@@ -892,6 +883,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.71eaa9b8d1160b47b16fe7e7df5da03043290604cfcd4d16257cd4b48cfdf547.eb6657c3c1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-15T11:24:05Z</t>
+  </si>
+  <si>
+    <t>96c421dc913607f4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.1866efeba6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1639,11 +1639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T872"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="D43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1916,19 +1916,19 @@
         <v>19</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F10" s="13">
         <v>45267</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>23</v>
@@ -1962,7 +1962,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
@@ -2000,7 +2000,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
@@ -2038,7 +2038,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="14"/>
@@ -2082,10 +2082,10 @@
         <v>45267</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>46</v>
@@ -2101,7 +2101,7 @@
         <v>41</v>
       </c>
       <c r="N14" s="37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O14" s="37" t="s">
         <v>23</v>
@@ -2138,10 +2138,10 @@
         <v>45267</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>46</v>
@@ -2157,7 +2157,7 @@
         <v>41</v>
       </c>
       <c r="N15" s="37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O15" s="37" t="s">
         <v>23</v>
@@ -2194,7 +2194,7 @@
         <v>45267</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2209,7 +2209,7 @@
         <v>41</v>
       </c>
       <c r="N16" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O16" s="37" t="s">
         <v>23</v>
@@ -2242,19 +2242,19 @@
         <v>27</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F17" s="13">
         <v>45267</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>23</v>
@@ -2267,7 +2267,7 @@
         <v>41</v>
       </c>
       <c r="N17" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O17" s="37" t="s">
         <v>23</v>
@@ -2298,16 +2298,16 @@
         <v>28</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F18" s="13">
         <v>45267</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>46</v>
@@ -2323,7 +2323,7 @@
         <v>41</v>
       </c>
       <c r="N18" s="47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O18" s="37" t="s">
         <v>23</v>
@@ -2356,19 +2356,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F19" s="13">
         <v>45267</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J19" s="15" t="s">
         <v>23</v>
@@ -2381,7 +2381,7 @@
         <v>41</v>
       </c>
       <c r="N19" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O19" s="37" t="s">
         <v>23</v>
@@ -2412,7 +2412,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F20" s="55"/>
       <c r="G20" s="14"/>
@@ -2450,19 +2450,19 @@
         <v>31</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F21" s="13">
         <v>45267</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J21" s="15" t="s">
         <v>23</v>
@@ -2475,7 +2475,7 @@
         <v>41</v>
       </c>
       <c r="N21" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O21" s="37" t="s">
         <v>23</v>
@@ -2506,19 +2506,19 @@
         <v>32</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F22" s="13">
         <v>45267</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>23</v>
@@ -2531,7 +2531,7 @@
         <v>41</v>
       </c>
       <c r="N22" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O22" s="37" t="s">
         <v>23</v>
@@ -2562,19 +2562,19 @@
         <v>33</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F23" s="13">
         <v>45267</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J23" s="15" t="s">
         <v>23</v>
@@ -2587,7 +2587,7 @@
         <v>41</v>
       </c>
       <c r="N23" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O23" s="37" t="s">
         <v>23</v>
@@ -2618,19 +2618,19 @@
         <v>34</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F24" s="13">
         <v>45267</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>23</v>
@@ -2643,7 +2643,7 @@
         <v>41</v>
       </c>
       <c r="N24" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O24" s="37" t="s">
         <v>23</v>
@@ -2674,7 +2674,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="14"/>
@@ -2712,7 +2712,7 @@
         <v>36</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
@@ -2750,19 +2750,19 @@
         <v>37</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F27" s="13">
         <v>45267</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J27" s="15" t="s">
         <v>23</v>
@@ -2775,7 +2775,7 @@
         <v>41</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O27" s="37" t="s">
         <v>23</v>
@@ -2804,7 +2804,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
@@ -2848,10 +2848,10 @@
         <v>45258</v>
       </c>
       <c r="G29" s="36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I29" s="36" t="s">
         <v>46</v>
@@ -2867,7 +2867,7 @@
         <v>41</v>
       </c>
       <c r="N29" s="37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O29" s="37" t="s">
         <v>23</v>
@@ -2904,10 +2904,10 @@
         <v>45258</v>
       </c>
       <c r="G30" s="36" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I30" s="36" t="s">
         <v>46</v>
@@ -2923,7 +2923,7 @@
         <v>41</v>
       </c>
       <c r="N30" s="37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O30" s="37" t="s">
         <v>23</v>
@@ -2975,7 +2975,7 @@
         <v>41</v>
       </c>
       <c r="N31" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O31" s="37" t="s">
         <v>23</v>
@@ -3191,7 +3191,7 @@
         <v>41</v>
       </c>
       <c r="N36" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O36" s="47" t="s">
         <v>23</v>
@@ -3247,7 +3247,7 @@
         <v>41</v>
       </c>
       <c r="N37" s="47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O37" s="47" t="s">
         <v>23</v>
@@ -3303,7 +3303,7 @@
         <v>41</v>
       </c>
       <c r="N38" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O38" s="47" t="s">
         <v>23</v>
@@ -3397,7 +3397,7 @@
         <v>41</v>
       </c>
       <c r="N40" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O40" s="47" t="s">
         <v>23</v>
@@ -3453,7 +3453,7 @@
         <v>41</v>
       </c>
       <c r="N41" s="47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O41" s="47" t="s">
         <v>23</v>
@@ -3509,7 +3509,7 @@
         <v>41</v>
       </c>
       <c r="N42" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O42" s="47" t="s">
         <v>23</v>
@@ -3565,7 +3565,7 @@
         <v>41</v>
       </c>
       <c r="N43" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O43" s="47" t="s">
         <v>23</v>
@@ -3621,7 +3621,7 @@
         <v>41</v>
       </c>
       <c r="N44" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O44" s="47" t="s">
         <v>23</v>
@@ -3677,7 +3677,7 @@
         <v>41</v>
       </c>
       <c r="N45" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O45" s="47" t="s">
         <v>23</v>
@@ -3711,16 +3711,16 @@
         <v>94</v>
       </c>
       <c r="F46" s="35">
-        <v>45252</v>
+        <v>45275</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="H46" s="36" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="J46" s="37" t="s">
         <v>23</v>
@@ -3733,7 +3733,7 @@
         <v>41</v>
       </c>
       <c r="N46" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O46" s="47" t="s">
         <v>23</v>
@@ -3808,13 +3808,13 @@
         <v>45252</v>
       </c>
       <c r="G48" s="36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H48" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I48" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J48" s="37" t="s">
         <v>23</v>
@@ -3827,7 +3827,7 @@
         <v>41</v>
       </c>
       <c r="N48" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O48" s="47" t="s">
         <v>23</v>
@@ -4054,13 +4054,13 @@
         <v>45252</v>
       </c>
       <c r="G54" s="36" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H54" s="36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I54" s="36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J54" s="37" t="s">
         <v>23</v>
@@ -4073,7 +4073,7 @@
         <v>41</v>
       </c>
       <c r="N54" s="54" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O54" s="47" t="s">
         <v>23</v>
@@ -4101,22 +4101,22 @@
         <v>18</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F55" s="35">
         <v>45257</v>
       </c>
       <c r="G55" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H55" s="36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I55" s="36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J55" s="37" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Fix test 64, 152
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/2.0/report-checklist.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="217">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -581,12 +581,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.45c976e65f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-22T16:25:58Z</t>
-  </si>
-  <si>
-    <t>12331bad019decf1</t>
-  </si>
-  <si>
     <t>2023-11-22T16:29:53Z</t>
   </si>
   <si>
@@ -822,12 +816,6 @@
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.71eaa9b8d1160b47b16fe7e7df5da03043290604cfcd4d16257cd4b48cfdf547.0f13fcf3d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-12-07T11:20:31Z</t>
-  </si>
-  <si>
-    <t>96c02136abf4a79d</t>
-  </si>
-  <si>
     <t>2023-12-07T11:23:14Z</t>
   </si>
   <si>
@@ -892,6 +880,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.1866efeba6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-18T15:18:29Z</t>
+  </si>
+  <si>
+    <t>9a2e360c36ab6fa6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.f06c5d644b174866d34fe90792ae247ee60a93e8939c3c723328ebda12069b69.a5e668b7a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-18T15:15:33Z</t>
+  </si>
+  <si>
+    <t>7dfe66e02df2ca1b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.71eaa9b8d1160b47b16fe7e7df5da03043290604cfcd4d16257cd4b48cfdf547.222cae515f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1640,10 +1646,10 @@
   <dimension ref="A1:T872"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1916,19 +1922,19 @@
         <v>19</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F10" s="13">
         <v>45267</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>23</v>
@@ -1962,7 +1968,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
@@ -2000,7 +2006,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
@@ -2038,7 +2044,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="14"/>
@@ -2082,10 +2088,10 @@
         <v>45267</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>46</v>
@@ -2101,7 +2107,7 @@
         <v>41</v>
       </c>
       <c r="N14" s="37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O14" s="37" t="s">
         <v>23</v>
@@ -2138,10 +2144,10 @@
         <v>45267</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>46</v>
@@ -2157,7 +2163,7 @@
         <v>41</v>
       </c>
       <c r="N15" s="37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O15" s="37" t="s">
         <v>23</v>
@@ -2194,7 +2200,7 @@
         <v>45267</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2209,7 +2215,7 @@
         <v>41</v>
       </c>
       <c r="N16" s="37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O16" s="37" t="s">
         <v>23</v>
@@ -2242,19 +2248,19 @@
         <v>27</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F17" s="13">
         <v>45267</v>
       </c>
       <c r="G17" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="I17" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>190</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>23</v>
@@ -2267,7 +2273,7 @@
         <v>41</v>
       </c>
       <c r="N17" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O17" s="37" t="s">
         <v>23</v>
@@ -2298,19 +2304,19 @@
         <v>28</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F18" s="13">
-        <v>45267</v>
+        <v>45278</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>23</v>
@@ -2356,19 +2362,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F19" s="13">
         <v>45267</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J19" s="15" t="s">
         <v>23</v>
@@ -2381,7 +2387,7 @@
         <v>41</v>
       </c>
       <c r="N19" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O19" s="37" t="s">
         <v>23</v>
@@ -2412,7 +2418,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F20" s="55"/>
       <c r="G20" s="14"/>
@@ -2450,19 +2456,19 @@
         <v>31</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F21" s="13">
         <v>45267</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J21" s="15" t="s">
         <v>23</v>
@@ -2475,7 +2481,7 @@
         <v>41</v>
       </c>
       <c r="N21" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O21" s="37" t="s">
         <v>23</v>
@@ -2506,19 +2512,19 @@
         <v>32</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F22" s="13">
         <v>45267</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>23</v>
@@ -2531,7 +2537,7 @@
         <v>41</v>
       </c>
       <c r="N22" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O22" s="37" t="s">
         <v>23</v>
@@ -2562,19 +2568,19 @@
         <v>33</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F23" s="13">
         <v>45267</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J23" s="15" t="s">
         <v>23</v>
@@ -2587,7 +2593,7 @@
         <v>41</v>
       </c>
       <c r="N23" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O23" s="37" t="s">
         <v>23</v>
@@ -2618,19 +2624,19 @@
         <v>34</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F24" s="13">
         <v>45267</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>23</v>
@@ -2643,7 +2649,7 @@
         <v>41</v>
       </c>
       <c r="N24" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O24" s="37" t="s">
         <v>23</v>
@@ -2674,7 +2680,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="14"/>
@@ -2712,7 +2718,7 @@
         <v>36</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
@@ -2750,19 +2756,19 @@
         <v>37</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F27" s="13">
         <v>45267</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J27" s="15" t="s">
         <v>23</v>
@@ -2775,7 +2781,7 @@
         <v>41</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O27" s="37" t="s">
         <v>23</v>
@@ -2804,7 +2810,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
@@ -2848,10 +2854,10 @@
         <v>45258</v>
       </c>
       <c r="G29" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" s="36" t="s">
         <v>160</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>162</v>
       </c>
       <c r="I29" s="36" t="s">
         <v>46</v>
@@ -2867,7 +2873,7 @@
         <v>41</v>
       </c>
       <c r="N29" s="37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O29" s="37" t="s">
         <v>23</v>
@@ -2904,10 +2910,10 @@
         <v>45258</v>
       </c>
       <c r="G30" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="H30" s="36" t="s">
-        <v>163</v>
       </c>
       <c r="I30" s="36" t="s">
         <v>46</v>
@@ -2923,7 +2929,7 @@
         <v>41</v>
       </c>
       <c r="N30" s="37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O30" s="37" t="s">
         <v>23</v>
@@ -2975,7 +2981,7 @@
         <v>41</v>
       </c>
       <c r="N31" s="37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O31" s="37" t="s">
         <v>23</v>
@@ -3191,7 +3197,7 @@
         <v>41</v>
       </c>
       <c r="N36" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O36" s="47" t="s">
         <v>23</v>
@@ -3225,16 +3231,16 @@
         <v>76</v>
       </c>
       <c r="F37" s="45">
-        <v>45252</v>
+        <v>45278</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="H37" s="36" t="s">
-        <v>123</v>
+        <v>212</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>46</v>
+        <v>213</v>
       </c>
       <c r="J37" s="47" t="s">
         <v>23</v>
@@ -3284,13 +3290,13 @@
         <v>45252</v>
       </c>
       <c r="G38" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="36" t="s">
         <v>124</v>
-      </c>
-      <c r="H38" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="I38" s="36" t="s">
-        <v>126</v>
       </c>
       <c r="J38" s="37" t="s">
         <v>23</v>
@@ -3303,7 +3309,7 @@
         <v>41</v>
       </c>
       <c r="N38" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O38" s="47" t="s">
         <v>23</v>
@@ -3378,13 +3384,13 @@
         <v>45252</v>
       </c>
       <c r="G40" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="I40" s="36" t="s">
         <v>127</v>
-      </c>
-      <c r="H40" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="I40" s="36" t="s">
-        <v>129</v>
       </c>
       <c r="J40" s="37" t="s">
         <v>23</v>
@@ -3397,7 +3403,7 @@
         <v>41</v>
       </c>
       <c r="N40" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O40" s="47" t="s">
         <v>23</v>
@@ -3434,13 +3440,13 @@
         <v>45252</v>
       </c>
       <c r="G41" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="I41" s="36" t="s">
         <v>130</v>
-      </c>
-      <c r="H41" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="I41" s="36" t="s">
-        <v>132</v>
       </c>
       <c r="J41" s="37" t="s">
         <v>23</v>
@@ -3453,7 +3459,7 @@
         <v>41</v>
       </c>
       <c r="N41" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O41" s="47" t="s">
         <v>23</v>
@@ -3490,13 +3496,13 @@
         <v>45252</v>
       </c>
       <c r="G42" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="I42" s="36" t="s">
         <v>133</v>
-      </c>
-      <c r="H42" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="I42" s="36" t="s">
-        <v>135</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>23</v>
@@ -3509,7 +3515,7 @@
         <v>41</v>
       </c>
       <c r="N42" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O42" s="47" t="s">
         <v>23</v>
@@ -3546,13 +3552,13 @@
         <v>45252</v>
       </c>
       <c r="G43" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I43" s="36" t="s">
         <v>136</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>138</v>
       </c>
       <c r="J43" s="37" t="s">
         <v>23</v>
@@ -3565,7 +3571,7 @@
         <v>41</v>
       </c>
       <c r="N43" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O43" s="47" t="s">
         <v>23</v>
@@ -3602,13 +3608,13 @@
         <v>45252</v>
       </c>
       <c r="G44" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="H44" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="I44" s="36" t="s">
         <v>139</v>
-      </c>
-      <c r="H44" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="I44" s="36" t="s">
-        <v>141</v>
       </c>
       <c r="J44" s="37" t="s">
         <v>23</v>
@@ -3621,7 +3627,7 @@
         <v>41</v>
       </c>
       <c r="N44" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O44" s="47" t="s">
         <v>23</v>
@@ -3658,13 +3664,13 @@
         <v>45252</v>
       </c>
       <c r="G45" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="I45" s="36" t="s">
         <v>142</v>
-      </c>
-      <c r="H45" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="I45" s="36" t="s">
-        <v>144</v>
       </c>
       <c r="J45" s="37" t="s">
         <v>23</v>
@@ -3677,7 +3683,7 @@
         <v>41</v>
       </c>
       <c r="N45" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O45" s="47" t="s">
         <v>23</v>
@@ -3714,13 +3720,13 @@
         <v>45275</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H46" s="36" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J46" s="37" t="s">
         <v>23</v>
@@ -3733,7 +3739,7 @@
         <v>41</v>
       </c>
       <c r="N46" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O46" s="47" t="s">
         <v>23</v>
@@ -3808,13 +3814,13 @@
         <v>45252</v>
       </c>
       <c r="G48" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I48" s="36" t="s">
         <v>145</v>
-      </c>
-      <c r="H48" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" s="36" t="s">
-        <v>147</v>
       </c>
       <c r="J48" s="37" t="s">
         <v>23</v>
@@ -3827,7 +3833,7 @@
         <v>41</v>
       </c>
       <c r="N48" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O48" s="47" t="s">
         <v>23</v>
@@ -4054,13 +4060,13 @@
         <v>45252</v>
       </c>
       <c r="G54" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="H54" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="I54" s="36" t="s">
         <v>148</v>
-      </c>
-      <c r="H54" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="I54" s="36" t="s">
-        <v>150</v>
       </c>
       <c r="J54" s="37" t="s">
         <v>23</v>
@@ -4073,7 +4079,7 @@
         <v>41</v>
       </c>
       <c r="N54" s="54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O54" s="47" t="s">
         <v>23</v>
@@ -4101,22 +4107,22 @@
         <v>18</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F55" s="35">
         <v>45257</v>
       </c>
       <c r="G55" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="H55" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="I55" s="36" t="s">
         <v>153</v>
-      </c>
-      <c r="H55" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="I55" s="36" t="s">
-        <v>155</v>
       </c>
       <c r="J55" s="37" t="s">
         <v>23</v>

</xml_diff>